<commit_message>
contact us page updated
</commit_message>
<xml_diff>
--- a/backend/data/contact_us.xlsx
+++ b/backend/data/contact_us.xlsx
@@ -3,6 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500"/>
+  </bookViews>
   <sheets>
     <sheet sheetId="1" name="contact_us" state="visible" r:id="rId4"/>
   </sheets>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -19,7 +22,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>subject</t>
+    <t>Subject</t>
   </si>
   <si>
     <t>Message</t>
@@ -35,6 +38,84 @@
   </si>
   <si>
     <t>hello I would like to contact you</t>
+  </si>
+  <si>
+    <t>Akshay</t>
+  </si>
+  <si>
+    <t>akshay@gmail.com</t>
+  </si>
+  <si>
+    <t>To contact the admin</t>
+  </si>
+  <si>
+    <t>I just want to conatct the admin</t>
+  </si>
+  <si>
+    <t>Akshay Kumar S</t>
+  </si>
+  <si>
+    <t>akshaykumars9108@gmail.com</t>
+  </si>
+  <si>
+    <t>To contact the Admin</t>
+  </si>
+  <si>
+    <t>I want to sell my artwork on this Artify website</t>
+  </si>
+  <si>
+    <t>Reddy</t>
+  </si>
+  <si>
+    <t>reddy@gmail.com</t>
+  </si>
+  <si>
+    <t>To buy an artwork</t>
+  </si>
+  <si>
+    <t>Can you guide me to buy a new portrait artwork?</t>
+  </si>
+  <si>
+    <t>Aishwarya</t>
+  </si>
+  <si>
+    <t>aishwarya@gmail.com</t>
+  </si>
+  <si>
+    <t>To contact the Artist</t>
+  </si>
+  <si>
+    <t>I just want to contact artist named Akshay Kumar S.</t>
+  </si>
+  <si>
+    <t>Kaushik</t>
+  </si>
+  <si>
+    <t>kaushik@gmail.com</t>
+  </si>
+  <si>
+    <t>To buy artwork</t>
+  </si>
+  <si>
+    <t>I want to buy artworks to compete in art competition at our school</t>
+  </si>
+  <si>
+    <t>Darshan</t>
+  </si>
+  <si>
+    <t>darshan@gmail.com</t>
+  </si>
+  <si>
+    <t>I want to create an account in Artify</t>
+  </si>
+  <si>
+    <t>Shankar Shettigar</t>
+  </si>
+  <si>
+    <t>shankar@gmail.com</t>
+  </si>
+  <si>
+    <t>I want to buy digital paintings of lord Ganesha</t>
   </si>
 </sst>
 </file>
@@ -411,8 +492,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -442,8 +534,106 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>